<commit_message>
Update timer feature and logic
</commit_message>
<xml_diff>
--- a/test_system/uploads/Book1.xlsx
+++ b/test_system/uploads/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XAMPP\htdocs\test_system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\badhu\OneDrive\Pictures\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56396D45-FC6C-46A6-A950-C8E09DBDE1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FD10BDC-6B6E-42DC-ACB9-6F7808DBBADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{588BA949-F2C1-43B0-B9BB-C24DB0D11CD6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D17FE04A-2115-430F-BEFC-4E0BB7019F56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,36 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>SCQ</t>
+  </si>
+  <si>
+    <t>What will be the maximum value of any analog input in case of a 12 bit AI module?</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>FILL</t>
+  </si>
+  <si>
+    <t>INDIAS CAPITAl?</t>
+  </si>
   <si>
     <t>Q. No</t>
   </si>
@@ -51,77 +75,24 @@
     <t>correct_asnwer</t>
   </si>
   <si>
-    <t>Fill</t>
-  </si>
-  <si>
-    <t>WinCC stands for</t>
-  </si>
-  <si>
-    <t>Win Credit Card</t>
-  </si>
-  <si>
-    <t>MCQ</t>
-  </si>
-  <si>
-    <t>How many types of Wincc projects are we can configure?</t>
-  </si>
-  <si>
-    <t>ONE</t>
-  </si>
-  <si>
-    <t>TWO</t>
-  </si>
-  <si>
-    <t>THREE</t>
-  </si>
-  <si>
-    <t>FOUR</t>
-  </si>
-  <si>
-    <t>Where to define start-up picture?</t>
-  </si>
-  <si>
-    <t>Graphics Designer</t>
-  </si>
-  <si>
-    <t>Computer Option</t>
-  </si>
-  <si>
-    <t>Both above</t>
-  </si>
-  <si>
-    <t>None of the above</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Full form of WinCC RC?</t>
-  </si>
-  <si>
-    <t>A, B</t>
-  </si>
-  <si>
-    <t>SCQ</t>
-  </si>
-  <si>
-    <t>T/F</t>
+    <t>4095</t>
+  </si>
+  <si>
+    <t>4096</t>
+  </si>
+  <si>
+    <t>2048</t>
+  </si>
+  <si>
+    <t>2046</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -149,23 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,189 +436,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E733CD88-5765-46EF-B8A2-1C18C14D5B15}">
-  <dimension ref="A1:H21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0E25347-ABEA-4F7C-AC8A-A6EFCE370902}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="3"/>
-    <col min="3" max="3" width="67.44140625" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="5" width="29.109375" customWidth="1"/>
-    <col min="6" max="6" width="25.77734375" customWidth="1"/>
-    <col min="7" max="7" width="29.21875" customWidth="1"/>
-    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+      <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>